<commit_message>
Modified examples and instructions for year 2018.
</commit_message>
<xml_diff>
--- a/se/Exempel.xlsx
+++ b/se/Exempel.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="120" yWindow="150" windowWidth="21075" windowHeight="10560"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Exempel" sheetId="1" r:id="rId1"/>
+    <sheet name="Kommunala skattesatser 2018" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Grundavdrag</t>
   </si>
@@ -27,12 +27,6 @@
     <t>Inkomst efter grundavdrag</t>
   </si>
   <si>
-    <t>Stockholms län</t>
-  </si>
-  <si>
-    <t>I Stockholm</t>
-  </si>
-  <si>
     <t>Grund för statlig inkomstskatt</t>
   </si>
   <si>
@@ -42,29 +36,68 @@
     <t>Grund för värnskatt</t>
   </si>
   <si>
-    <t>Västerbottens  län</t>
-  </si>
-  <si>
-    <t>I Västerbotten</t>
-  </si>
-  <si>
     <t>Exempel på olika skattesatser</t>
   </si>
   <si>
-    <t>Skattesatser</t>
-  </si>
-  <si>
     <t>Brytpunkt för statlig inkomstskatt</t>
   </si>
   <si>
     <t>Brytpunkt för värnskatt</t>
+  </si>
+  <si>
+    <t>Kommun</t>
+  </si>
+  <si>
+    <t>Ale</t>
+  </si>
+  <si>
+    <t>Bergs</t>
+  </si>
+  <si>
+    <t>Botkyrka</t>
+  </si>
+  <si>
+    <t>Danderyd</t>
+  </si>
+  <si>
+    <t>Falu</t>
+  </si>
+  <si>
+    <t>Gotlands</t>
+  </si>
+  <si>
+    <t>Halmstads</t>
+  </si>
+  <si>
+    <t>Kalix</t>
+  </si>
+  <si>
+    <t>Mora</t>
+  </si>
+  <si>
+    <t>Orsa</t>
+  </si>
+  <si>
+    <t>Stockholms</t>
+  </si>
+  <si>
+    <t>Uppsala</t>
+  </si>
+  <si>
+    <t>Vilhelmina</t>
+  </si>
+  <si>
+    <t>I Stockholms kommun</t>
+  </si>
+  <si>
+    <t>I Vilhelmina kommunn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +128,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,11 +161,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -126,6 +184,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,12 +502,17 @@
     <col min="4" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="9">
+        <v>2018</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>13100</v>
+        <v>13400</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -453,14 +520,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6">
-        <v>413200</v>
+        <v>455300</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" s="7">
         <v>0.2</v>
@@ -468,14 +535,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>591600</v>
+        <v>662300</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" s="7">
         <v>0.05</v>
@@ -483,7 +550,7 @@
     </row>
     <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -491,22 +558,27 @@
         <v>1</v>
       </c>
       <c r="B9" s="4">
-        <v>13100</v>
+        <f>B2</f>
+        <v>13400</v>
       </c>
       <c r="C9" s="4">
-        <v>13101</v>
+        <f>B2+1</f>
+        <v>13401</v>
       </c>
       <c r="D9" s="4">
-        <v>426300</v>
+        <f>B2+B3</f>
+        <v>468700</v>
       </c>
       <c r="E9" s="4">
-        <v>426301</v>
+        <f>$B$2+$B$3+1</f>
+        <v>468701</v>
       </c>
       <c r="F9" s="4">
         <v>500000</v>
       </c>
       <c r="G9" s="4">
-        <v>604701</v>
+        <f>$B$2+$B$4+1</f>
+        <v>675701</v>
       </c>
       <c r="H9" s="4">
         <v>700000</v>
@@ -526,28 +598,28 @@
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>413200</v>
+        <v>455300</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>413201</v>
+        <v>455301</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>486900</v>
+        <f>F9-$B$2</f>
+        <v>486600</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>591601</v>
+        <v>662301</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>686900</v>
+        <f>H9-$B$2</f>
+        <v>686600</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" ref="B11:H11" si="1">IF(B10&gt;$B$3,B10-$B$3,0)</f>
@@ -566,21 +638,21 @@
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
-        <v>73700</v>
+        <f>IF(F10&gt;$B$3,F10-$B$3,0)</f>
+        <v>31300</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>178401</v>
+        <v>207001</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>273700</v>
+        <f>IF(H10&gt;$B$3,H10-$B$3,0)</f>
+        <v>231300</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" s="4">
         <f>IF(B10&gt;$B$4,B10-$B$42,0)</f>
@@ -608,7 +680,7 @@
       </c>
       <c r="H12" s="4">
         <f>IF(H10&gt;$B$4,H10-$B$4,0)</f>
-        <v>95300</v>
+        <v>24300</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -623,68 +695,68 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4">
-        <f>B$10*$B$20+B$11*$E$3+B$12*$E$4</f>
+        <f>B$10*'Kommunala skattesatser 2018'!$B$12+B$11*$E$3+B$12*$E$4</f>
         <v>0</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:H14" si="2">C10*$B$20+C11*$E$3+C12*$E$4</f>
-        <v>0.3039</v>
+        <f>C$10*'Kommunala skattesatser 2018'!$B$12+C$11*$E$3+C$12*$E$4</f>
+        <v>0.29980000000000001</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="2"/>
-        <v>125571.48</v>
+        <f>D$10*'Kommunala skattesatser 2018'!$B$12+D$11*$E$3+D$12*$E$4</f>
+        <v>136498.94</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
-        <v>125571.98389999999</v>
+        <f>E$10*'Kommunala skattesatser 2018'!$B$12+E$11*$E$3+E$12*$E$4</f>
+        <v>136499.43980000002</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="2"/>
-        <v>162708.91</v>
+        <f>F$10*'Kommunala skattesatser 2018'!$B$12+F$11*$E$3+F$12*$E$4</f>
+        <v>152142.68</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="2"/>
-        <v>215467.79389999999</v>
+        <f>G$10*'Kommunala skattesatser 2018'!$B$12+G$11*$E$3+G$12*$E$4</f>
+        <v>239958.08980000002</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="2"/>
-        <v>268253.91000000003</v>
+        <f>H$10*'Kommunala skattesatser 2018'!$B$12+H$11*$E$3+H$12*$E$4</f>
+        <v>253317.68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" ref="B15:H15" si="3">B$10*$B$21+B$11*$E$3+B$12*$E$4</f>
+        <f>B$10*'Kommunala skattesatser 2018'!$B$14+B$11*$E$3+B$12*$E$4</f>
         <v>0</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="3"/>
-        <v>0.33139999999999997</v>
+        <f>C$10*'Kommunala skattesatser 2018'!$B$14+C$11*$E$3+C$12*$E$4</f>
+        <v>0.34749999999999998</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="3"/>
-        <v>136934.47999999998</v>
+        <f>D$10*'Kommunala skattesatser 2018'!$B$14+D$11*$E$3+D$12*$E$4</f>
+        <v>158216.75</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="3"/>
-        <v>136935.01139999999</v>
+        <f>E$10*'Kommunala skattesatser 2018'!$B$14+E$11*$E$3+E$12*$E$4</f>
+        <v>158217.29749999999</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="3"/>
-        <v>176098.65999999997</v>
+        <f>F$10*'Kommunala skattesatser 2018'!$B$14+F$11*$E$3+F$12*$E$4</f>
+        <v>175353.5</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="3"/>
-        <v>231736.82139999999</v>
+        <f>G$10*'Kommunala skattesatser 2018'!$B$14+G$11*$E$3+G$12*$E$4</f>
+        <v>271549.84749999997</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="3"/>
-        <v>287143.65999999997</v>
+        <f>H$10*'Kommunala skattesatser 2018'!$B$14+H$11*$E$3+H$12*$E$4</f>
+        <v>286068.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,30 +772,20 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="8">
-        <v>0.3039</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="8">
-        <v>0.33139999999999997</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,12 +801,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.33550000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.3372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.32229999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.29430000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.33889999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0.3397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0.34050000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.29980000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.32819999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.34749999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -753,7 +934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>